<commit_message>
Change fiducial points as specified in https://jira.stsci.edu/browse/JWSTSIAF-163 FGS1_FULL V2Ref = 206.464 V3Ref = -697.970
FGS2_FULL
V2Ref = 22.845
V3Ref = -699.489
</commit_message>
<xml_diff>
--- a/pysiaf/pre_delivery_data/FGS/FGS_SIAF.xlsx
+++ b/pysiaf/pre_delivery_data/FGS/FGS_SIAF.xlsx
@@ -416,10 +416,10 @@
     <t>0.07005886361899759</t>
   </si>
   <si>
-    <t>206.441</t>
-  </si>
-  <si>
-    <t>-698.069</t>
+    <t>206.464</t>
+  </si>
+  <si>
+    <t>-697.97</t>
   </si>
   <si>
     <t>-1.2508171328901623</t>
@@ -833,10 +833,10 @@
     <t>0.06982049767478168</t>
   </si>
   <si>
-    <t>22.818</t>
-  </si>
-  <si>
-    <t>-699.591</t>
+    <t>22.845</t>
+  </si>
+  <si>
+    <t>-699.489</t>
   </si>
   <si>
     <t>0.19027904463505274</t>
@@ -1148,10 +1148,10 @@
     <t>0.06826328566738032</t>
   </si>
   <si>
-    <t>140.22320831759697</t>
-  </si>
-  <si>
-    <t>-631.6031421040232</t>
+    <t>140.24620831759697</t>
+  </si>
+  <si>
+    <t>-631.5041421040232</t>
   </si>
   <si>
     <t>-90.11986052827177</t>
@@ -1304,10 +1304,10 @@
     <t>0.0690519661730757</t>
   </si>
   <si>
-    <t>173.09754992847954</t>
-  </si>
-  <si>
-    <t>-664.5439857996336</t>
+    <t>173.12054992847953</t>
+  </si>
+  <si>
+    <t>-664.4449857996336</t>
   </si>
   <si>
     <t>-89.88292140149322</t>
@@ -1661,10 +1661,10 @@
     <t>0.07243013316055126</t>
   </si>
   <si>
-    <t>-43.85131407447644</t>
-  </si>
-  <si>
-    <t>-769.0640793115072</t>
+    <t>-43.82431407447644</t>
+  </si>
+  <si>
+    <t>-768.9620793115071</t>
   </si>
   <si>
     <t>-91.55024882984965</t>
@@ -1814,10 +1814,10 @@
     <t>0.07098031503333774</t>
   </si>
   <si>
-    <t>-10.195802478181784</t>
-  </si>
-  <si>
-    <t>-733.8989381342564</t>
+    <t>-10.168802478181787</t>
+  </si>
+  <si>
+    <t>-733.7969381342564</t>
   </si>
   <si>
     <t>-91.10127545516434</t>
@@ -2168,10 +2168,10 @@
     <t>0.07012186595013008</t>
   </si>
   <si>
-    <t>207.27466130057243</t>
-  </si>
-  <si>
-    <t>-700.1422770413226</t>
+    <t>207.29766130057243</t>
+  </si>
+  <si>
+    <t>-700.0432770413227</t>
   </si>
   <si>
     <t>-71.03733744343728</t>
@@ -2327,10 +2327,10 @@
     <t>0.07193042652028452</t>
   </si>
   <si>
-    <t>144.33150295264775</t>
-  </si>
-  <si>
-    <t>-763.2005356668122</t>
+    <t>144.35450295264775</t>
+  </si>
+  <si>
+    <t>-763.1015356668123</t>
   </si>
   <si>
     <t>-135.34200519876435</t>
@@ -2486,10 +2486,10 @@
     <t>0.07173234893063828</t>
   </si>
   <si>
-    <t>259.95730166328474</t>
-  </si>
-  <si>
-    <t>-739.4292610098595</t>
+    <t>259.98030166328476</t>
+  </si>
+  <si>
+    <t>-739.3302610098596</t>
   </si>
   <si>
     <t>-19.224851721071236</t>
@@ -2645,10 +2645,10 @@
     <t>0.06894015219133763</t>
   </si>
   <si>
-    <t>269.24444287044804</t>
-  </si>
-  <si>
-    <t>-633.7170008127497</t>
+    <t>269.26744287044806</t>
+  </si>
+  <si>
+    <t>-633.6180008127498</t>
   </si>
   <si>
     <t>-7.632315416168646</t>
@@ -2798,10 +2798,10 @@
     <t>0.06832148202910197</t>
   </si>
   <si>
-    <t>141.9722760030966</t>
-  </si>
-  <si>
-    <t>-634.4336991945218</t>
+    <t>141.9952760030966</t>
+  </si>
+  <si>
+    <t>-634.3346991945218</t>
   </si>
   <si>
     <t>-134.88980025659524</t>
@@ -2954,10 +2954,10 @@
     <t>0.06980318033342428</t>
   </si>
   <si>
-    <t>23.737548440981122</t>
-  </si>
-  <si>
-    <t>-699.0553444181352</t>
+    <t>23.76454844098112</t>
+  </si>
+  <si>
+    <t>-698.9533444181352</t>
   </si>
   <si>
     <t>-69.20535467436002</t>
@@ -3110,10 +3110,10 @@
     <t>0.07147198586306203</t>
   </si>
   <si>
-    <t>-25.307612507901442</t>
-  </si>
-  <si>
-    <t>-746.1380353045871</t>
+    <t>-25.280612507901445</t>
+  </si>
+  <si>
+    <t>-746.0360353045871</t>
   </si>
   <si>
     <t>-118.093884031113</t>
@@ -3257,10 +3257,10 @@
     <t>0.07183087842299725</t>
   </si>
   <si>
-    <t>85.78358619356544</t>
-  </si>
-  <si>
-    <t>-764.3616144481065</t>
+    <t>85.81058619356544</t>
+  </si>
+  <si>
+    <t>-764.2596144481065</t>
   </si>
   <si>
     <t>-6.942777623204338</t>
@@ -3404,10 +3404,10 @@
     <t>0.0682484055679046</t>
   </si>
   <si>
-    <t>85.1083366991081</t>
-  </si>
-  <si>
-    <t>-635.3249698623604</t>
+    <t>85.1353366991081</t>
+  </si>
+  <si>
+    <t>-635.2229698623605</t>
   </si>
   <si>
     <t>-8.046552764412846</t>
@@ -3551,10 +3551,10 @@
     <t>0.068596053603498</t>
   </si>
   <si>
-    <t>-39.735127140954006</t>
-  </si>
-  <si>
-    <t>-636.6538148228858</t>
+    <t>-39.70812714095401</t>
+  </si>
+  <si>
+    <t>-636.5518148228857</t>
   </si>
   <si>
     <t>-132.88491507454154</t>

</xml_diff>

<commit_message>
Updating J-FRAME values from new OTE-01 mosaic
</commit_message>
<xml_diff>
--- a/pysiaf/pre_delivery_data/FGS/FGS_SIAF.xlsx
+++ b/pysiaf/pre_delivery_data/FGS/FGS_SIAF.xlsx
@@ -20319,17 +20319,17 @@
       </c>
       <c r="P35" s="3" t="inlineStr">
         <is>
-          <t>163.826</t>
+          <t>162.233</t>
         </is>
       </c>
       <c r="Q35" s="3" t="inlineStr">
         <is>
-          <t>177.606</t>
+          <t>171.991</t>
         </is>
       </c>
       <c r="R35" s="3" t="inlineStr">
         <is>
-          <t>0.00963132</t>
+          <t>0.009590215</t>
         </is>
       </c>
       <c r="S35" s="3" t="inlineStr">

</xml_diff>

<commit_message>
Changed _siaf_alignment.txt files for niriss and fgs, and ran generate scripts
</commit_message>
<xml_diff>
--- a/pysiaf/pre_delivery_data/FGS/FGS_SIAF.xlsx
+++ b/pysiaf/pre_delivery_data/FGS/FGS_SIAF.xlsx
@@ -2559,12 +2559,12 @@
       </c>
       <c r="P5" s="3" t="inlineStr">
         <is>
-          <t>22.835</t>
+          <t>22.865</t>
         </is>
       </c>
       <c r="Q5" s="3" t="inlineStr">
         <is>
-          <t>-699.423</t>
+          <t>-699.28</t>
         </is>
       </c>
       <c r="R5" s="3" t="inlineStr">
@@ -3151,12 +3151,12 @@
       </c>
       <c r="P6" s="3" t="inlineStr">
         <is>
-          <t>22.835</t>
+          <t>22.865</t>
         </is>
       </c>
       <c r="Q6" s="3" t="inlineStr">
         <is>
-          <t>-699.423</t>
+          <t>-699.28</t>
         </is>
       </c>
       <c r="R6" s="3" t="inlineStr">
@@ -9071,12 +9071,12 @@
       </c>
       <c r="P16" s="3" t="inlineStr">
         <is>
-          <t>-43.795554756956385</t>
+          <t>-43.76555475695639</t>
         </is>
       </c>
       <c r="Q16" s="3" t="inlineStr">
         <is>
-          <t>-768.6886154906737</t>
+          <t>-768.5456154906736</t>
         </is>
       </c>
       <c r="R16" s="3" t="inlineStr">
@@ -9663,12 +9663,12 @@
       </c>
       <c r="P17" s="3" t="inlineStr">
         <is>
-          <t>-10.181331515712449</t>
+          <t>-10.151331515712451</t>
         </is>
       </c>
       <c r="Q17" s="3" t="inlineStr">
         <is>
-          <t>-733.668328548254</t>
+          <t>-733.5253285482539</t>
         </is>
       </c>
       <c r="R17" s="3" t="inlineStr">
@@ -10255,12 +10255,12 @@
       </c>
       <c r="P18" s="3" t="inlineStr">
         <is>
-          <t>22.835</t>
+          <t>22.865</t>
         </is>
       </c>
       <c r="Q18" s="3" t="inlineStr">
         <is>
-          <t>-699.423</t>
+          <t>-699.28</t>
         </is>
       </c>
       <c r="R18" s="3" t="inlineStr">
@@ -10847,12 +10847,12 @@
       </c>
       <c r="P19" s="3" t="inlineStr">
         <is>
-          <t>-43.795554756956385</t>
+          <t>-43.76555475695639</t>
         </is>
       </c>
       <c r="Q19" s="3" t="inlineStr">
         <is>
-          <t>-768.6886154906737</t>
+          <t>-768.5456154906736</t>
         </is>
       </c>
       <c r="R19" s="3" t="inlineStr">
@@ -11439,12 +11439,12 @@
       </c>
       <c r="P20" s="3" t="inlineStr">
         <is>
-          <t>-10.181331515712449</t>
+          <t>-10.151331515712451</t>
         </is>
       </c>
       <c r="Q20" s="3" t="inlineStr">
         <is>
-          <t>-733.668328548254</t>
+          <t>-733.5253285482539</t>
         </is>
       </c>
       <c r="R20" s="3" t="inlineStr">
@@ -12031,12 +12031,12 @@
       </c>
       <c r="P21" s="3" t="inlineStr">
         <is>
-          <t>22.835</t>
+          <t>22.865</t>
         </is>
       </c>
       <c r="Q21" s="3" t="inlineStr">
         <is>
-          <t>-699.423</t>
+          <t>-699.28</t>
         </is>
       </c>
       <c r="R21" s="3" t="inlineStr">
@@ -12623,12 +12623,12 @@
       </c>
       <c r="P22" s="3" t="inlineStr">
         <is>
-          <t>-43.795554756956385</t>
+          <t>-43.76555475695639</t>
         </is>
       </c>
       <c r="Q22" s="3" t="inlineStr">
         <is>
-          <t>-768.6886154906737</t>
+          <t>-768.5456154906736</t>
         </is>
       </c>
       <c r="R22" s="3" t="inlineStr">
@@ -13215,12 +13215,12 @@
       </c>
       <c r="P23" s="3" t="inlineStr">
         <is>
-          <t>-10.181331515712449</t>
+          <t>-10.151331515712451</t>
         </is>
       </c>
       <c r="Q23" s="3" t="inlineStr">
         <is>
-          <t>-733.668328548254</t>
+          <t>-733.5253285482539</t>
         </is>
       </c>
       <c r="R23" s="3" t="inlineStr">
@@ -13807,12 +13807,12 @@
       </c>
       <c r="P24" s="3" t="inlineStr">
         <is>
-          <t>22.835</t>
+          <t>22.865</t>
         </is>
       </c>
       <c r="Q24" s="3" t="inlineStr">
         <is>
-          <t>-699.423</t>
+          <t>-699.28</t>
         </is>
       </c>
       <c r="R24" s="3" t="inlineStr">
@@ -17359,12 +17359,12 @@
       </c>
       <c r="P30" s="3" t="inlineStr">
         <is>
-          <t>23.75381501621084</t>
+          <t>23.783815016210838</t>
         </is>
       </c>
       <c r="Q30" s="3" t="inlineStr">
         <is>
-          <t>-698.8888585747162</t>
+          <t>-698.7458585747162</t>
         </is>
       </c>
       <c r="R30" s="3" t="inlineStr">
@@ -17951,12 +17951,12 @@
       </c>
       <c r="P31" s="3" t="inlineStr">
         <is>
-          <t>-25.28085550118208</t>
+          <t>-25.250855501182084</t>
         </is>
       </c>
       <c r="Q31" s="3" t="inlineStr">
         <is>
-          <t>-745.869442274178</t>
+          <t>-745.726442274178</t>
         </is>
       </c>
       <c r="R31" s="3" t="inlineStr">
@@ -18543,12 +18543,12 @@
       </c>
       <c r="P32" s="3" t="inlineStr">
         <is>
-          <t>85.55928499097821</t>
+          <t>85.58928499097821</t>
         </is>
       </c>
       <c r="Q32" s="3" t="inlineStr">
         <is>
-          <t>-764.2107063623097</t>
+          <t>-764.0677063623097</t>
         </is>
       </c>
       <c r="R32" s="3" t="inlineStr">
@@ -19135,12 +19135,12 @@
       </c>
       <c r="P33" s="3" t="inlineStr">
         <is>
-          <t>85.09128037693063</t>
+          <t>85.12128037693063</t>
         </is>
       </c>
       <c r="Q33" s="3" t="inlineStr">
         <is>
-          <t>-635.3400568092407</t>
+          <t>-635.1970568092406</t>
         </is>
       </c>
       <c r="R33" s="3" t="inlineStr">
@@ -19727,12 +19727,12 @@
       </c>
       <c r="P34" s="3" t="inlineStr">
         <is>
-          <t>-39.50841505022427</t>
+          <t>-39.47841505022427</t>
         </is>
       </c>
       <c r="Q34" s="3" t="inlineStr">
         <is>
-          <t>-636.4878219163089</t>
+          <t>-636.3448219163089</t>
         </is>
       </c>
       <c r="R34" s="3" t="inlineStr">
@@ -20319,17 +20319,17 @@
       </c>
       <c r="P35" s="3" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>180.255</t>
         </is>
       </c>
       <c r="Q35" s="3" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>175.783</t>
         </is>
       </c>
       <c r="R35" s="3" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>0.041688872</t>
         </is>
       </c>
       <c r="S35" s="3" t="inlineStr">
@@ -20841,7 +20841,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>J-FRAME</t>
+          <t>V-FRAME</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">

</xml_diff>